<commit_message>
Fixed some errors and some calculus were done
</commit_message>
<xml_diff>
--- a/Memory Map.xlsx
+++ b/Memory Map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeanPierre\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeanPierre\Desktop\Organizacion de computadores\Coffee-Star\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5085" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Variable</t>
   </si>
@@ -303,6 +303,18 @@
   </si>
   <si>
     <t>E75</t>
+  </si>
+  <si>
+    <t>E76-E77</t>
+  </si>
+  <si>
+    <t>Base gravable en UVTs</t>
+  </si>
+  <si>
+    <t>E78-E79</t>
+  </si>
+  <si>
+    <t>E7A-E7B</t>
   </si>
 </sst>
 </file>
@@ -707,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1293,6 +1305,45 @@
         <v>360</v>
       </c>
     </row>
+    <row r="72" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B74">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Fixed some bugs related with the function FTOI and decimals, ready to start testing
</commit_message>
<xml_diff>
--- a/Memory Map.xlsx
+++ b/Memory Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>Variable</t>
   </si>
@@ -315,6 +315,30 @@
   </si>
   <si>
     <t>E7A-E7B</t>
+  </si>
+  <si>
+    <t>E7C</t>
+  </si>
+  <si>
+    <t>Residuo de la cantidad de salarios</t>
+  </si>
+  <si>
+    <t>E7D</t>
+  </si>
+  <si>
+    <t>Residuo de la base gravable en UVTs</t>
+  </si>
+  <si>
+    <t>E7E</t>
+  </si>
+  <si>
+    <t>Cantidad de sueldos en entero</t>
+  </si>
+  <si>
+    <t>E7F</t>
+  </si>
+  <si>
+    <t>Cantidad de UVTs en base gravable en entero</t>
   </si>
 </sst>
 </file>
@@ -721,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1330,16 +1354,36 @@
       </c>
     </row>
     <row r="75" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="76" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
+      <c r="A76" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="77" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+      <c r="A77" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B77" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="79" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>

</xml_diff>